<commit_message>
Added new excel files, changed the tables from instrument and buyTickets. Insertion tables needs to be changed regarding excel files. Data in the excel tables is not totally completed
</commit_message>
<xml_diff>
--- a/Archivos Excel/instruments.xlsx
+++ b/Archivos Excel/instruments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\SkyDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79E4E64-E203-4A05-8CCF-223BEEE7AF7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB1486-4204-46E9-9403-62EAA495F68B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23940" windowHeight="9465" xr2:uid="{F097AE22-5C54-472A-BDF6-48EF6CA5434A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23940" windowHeight="9465" xr2:uid="{F097AE22-5C54-472A-BDF6-48EF6CA5434A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -420,189 +420,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E9E6B1-C716-4C8E-9EA7-407CC68D4912}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E18"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>6166844</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5334423</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4628696</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8484326</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5427651</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5264892</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5672350</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9452841</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5392301</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4136534</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7376429</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>7376429</v>
-      </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4949485</v>
-      </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4949365</v>
-      </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4949365</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5453651</v>
-      </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:E5"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="D12:E18"/>
+    <mergeCell ref="C1:D5"/>
+    <mergeCell ref="C7:D10"/>
+    <mergeCell ref="C12:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>